<commit_message>
Vorbereitung für 1 Meilenstein
</commit_message>
<xml_diff>
--- a/Literatur/T_Tools.xlsx
+++ b/Literatur/T_Tools.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3129315d83e5badf/Dokumente/GitHub/PS_InfoEng/Literatur/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Samardzic\Documents\GitHub\PS_InfoEng\Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A295B0-B30A-4B78-BF47-0479E71F1541}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E925EEB8-DC16-4A76-B76D-72457BA0CB41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11010" xr2:uid="{E514CA22-688F-4A54-BA34-1AB64F501A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>Usersicht</t>
   </si>
@@ -124,15 +119,29 @@
   <si>
     <t>Übertragbarkeit und Auswerung
 der Daten (niedrig, mittel, hoch)</t>
+  </si>
+  <si>
+    <t>Erhebungstools (Engere Auswahl)</t>
+  </si>
+  <si>
+    <t>Anbieter:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -393,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -401,18 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -489,6 +486,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -805,248 +815,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4E3E0D-6D55-467E-A865-F43D89624C67}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.73046875" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
-    <col min="3" max="3" width="20.59765625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="4" t="s">
+    <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="D6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="E6" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="29" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="D7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="E7" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="25" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="4" t="s">
+      <c r="D8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="18" t="s">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E11" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="18" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="D12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E12" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="18" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="D13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="E13" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
+      <c r="D14" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
+      <c r="D15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E16" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="24" t="s">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="D17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="E17" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="2" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="D19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>